<commit_message>
bulk data is all in
samples are on the way for composition analysis
</commit_message>
<xml_diff>
--- a/Data/CRCP Sediment Data Bulk Weight and Composition.xlsx
+++ b/Data/CRCP Sediment Data Bulk Weight and Composition.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" tabRatio="500" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" tabRatio="500" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Mar_2014" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="79">
   <si>
     <t>Pod(P)/Tube(T)</t>
   </si>
@@ -255,6 +255,18 @@
   <si>
     <t>NAN</t>
   </si>
+  <si>
+    <t>P2A-a</t>
+  </si>
+  <si>
+    <t>P2A-b</t>
+  </si>
+  <si>
+    <t>T1B-a</t>
+  </si>
+  <si>
+    <t>T1B-b</t>
+  </si>
 </sst>
 </file>
 
@@ -265,7 +277,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -349,6 +361,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13.2"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -463,7 +481,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -586,6 +604,15 @@
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -593,6 +620,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1067,16 +1097,16 @@
       <c r="A7" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="66" t="s">
+      <c r="B7" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="66"/>
-      <c r="D7" s="66"/>
-      <c r="F7" s="66" t="s">
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
+      <c r="F7" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="66"/>
-      <c r="H7" s="66"/>
+      <c r="G7" s="69"/>
+      <c r="H7" s="69"/>
     </row>
     <row r="8" spans="1:18" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
@@ -2200,8 +2230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+    <sheetView topLeftCell="A7" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2270,16 +2300,16 @@
       <c r="A7" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="66" t="s">
+      <c r="B7" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="66"/>
-      <c r="D7" s="66"/>
-      <c r="F7" s="66" t="s">
+      <c r="C7" s="72"/>
+      <c r="D7" s="72"/>
+      <c r="F7" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="66"/>
-      <c r="H7" s="66"/>
+      <c r="G7" s="72"/>
+      <c r="H7" s="72"/>
     </row>
     <row r="8" spans="1:12" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
@@ -2294,7 +2324,7 @@
       <c r="D8" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="29"/>
+      <c r="E8" s="66"/>
       <c r="F8" s="25" t="s">
         <v>1</v>
       </c>
@@ -2317,29 +2347,31 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="18">
-        <v>70.528000000000006</v>
-      </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="18">
-        <v>-70.528000000000006</v>
-      </c>
-      <c r="E9" s="13" t="str">
+      <c r="B9" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="67" t="str">
         <f>A9</f>
         <v>P1A</v>
       </c>
-      <c r="F9" s="18">
-        <v>1.6819999999999999</v>
-      </c>
-      <c r="G9" s="18">
-        <v>3.4660000000000002</v>
-      </c>
-      <c r="H9" s="18">
-        <v>1.784</v>
+      <c r="F9" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>24</v>
       </c>
       <c r="I9">
         <v>-14.290179999999999</v>
@@ -2356,29 +2388,31 @@
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B10" s="18">
         <v>110.10599999999999</v>
       </c>
-      <c r="C10" s="17"/>
+      <c r="C10" s="18">
+        <v>116.49</v>
+      </c>
       <c r="D10" s="18">
-        <v>-110.10599999999999</v>
-      </c>
-      <c r="E10" s="13" t="str">
+        <v>6.3840000000000003</v>
+      </c>
+      <c r="E10" s="67" t="str">
         <f t="shared" ref="E10:E27" si="1">A10</f>
         <v>P1B</v>
       </c>
       <c r="F10" s="18">
         <v>1.667</v>
       </c>
-      <c r="G10" s="18">
-        <v>2.552</v>
+      <c r="G10" s="68">
+        <v>2.5739999999999998</v>
       </c>
       <c r="H10" s="18">
-        <v>0.88500000000000001</v>
+        <v>0.90700000000000003</v>
       </c>
       <c r="I10">
         <v>-14.28941</v>
@@ -2395,29 +2429,31 @@
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B11" s="18">
         <v>112.16200000000001</v>
       </c>
-      <c r="C11" s="17"/>
+      <c r="C11" s="18">
+        <v>113.012</v>
+      </c>
       <c r="D11" s="18">
-        <v>-112.16200000000001</v>
-      </c>
-      <c r="E11" s="13" t="str">
+        <v>0.85</v>
+      </c>
+      <c r="E11" s="67" t="str">
         <f t="shared" si="1"/>
         <v>P1C</v>
       </c>
       <c r="F11" s="18">
         <v>1.738</v>
       </c>
-      <c r="G11" s="18">
-        <v>4.9089999999999998</v>
+      <c r="G11" s="68">
+        <v>4.4000000000000004</v>
       </c>
       <c r="H11" s="18">
-        <v>3.1709999999999998</v>
+        <v>2.6619999999999999</v>
       </c>
       <c r="I11">
         <v>-14.28833</v>
@@ -2434,29 +2470,31 @@
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B12" s="18">
         <v>69.935000000000002</v>
       </c>
-      <c r="C12" s="17"/>
+      <c r="C12" s="18">
+        <v>73.394999999999996</v>
+      </c>
       <c r="D12" s="18">
-        <v>-69.935000000000002</v>
-      </c>
-      <c r="E12" s="13" t="str">
+        <v>3.46</v>
+      </c>
+      <c r="E12" s="67" t="str">
         <f t="shared" si="1"/>
         <v>P2A</v>
       </c>
       <c r="F12" s="18">
         <v>1.615</v>
       </c>
-      <c r="G12" s="18">
-        <v>6.6520000000000001</v>
+      <c r="G12" s="68">
+        <v>6.3120000000000003</v>
       </c>
       <c r="H12" s="18">
-        <v>5.0369999999999999</v>
+        <v>4.6970000000000001</v>
       </c>
       <c r="I12">
         <v>-14.29177</v>
@@ -2473,29 +2511,31 @@
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B13" s="18">
         <v>113.377</v>
       </c>
-      <c r="C13" s="17"/>
+      <c r="C13" s="18">
+        <v>113.389</v>
+      </c>
       <c r="D13" s="18">
-        <v>-113.377</v>
-      </c>
-      <c r="E13" s="13" t="str">
+        <v>1.2E-2</v>
+      </c>
+      <c r="E13" s="67" t="str">
         <f t="shared" si="1"/>
         <v>P2B</v>
       </c>
       <c r="F13" s="18">
         <v>1.74</v>
       </c>
-      <c r="G13" s="18">
-        <v>1.7130000000000001</v>
+      <c r="G13" s="68">
+        <v>1.744</v>
       </c>
       <c r="H13" s="18">
-        <v>-2.7E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="I13">
         <v>-14.29142</v>
@@ -2512,29 +2552,31 @@
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B14" s="18">
         <v>67.063000000000002</v>
       </c>
-      <c r="C14" s="17"/>
+      <c r="C14" s="18">
+        <v>67.491</v>
+      </c>
       <c r="D14" s="18">
-        <v>-67.063000000000002</v>
-      </c>
-      <c r="E14" s="13" t="str">
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="E14" s="67" t="str">
         <f t="shared" si="1"/>
         <v>P2C</v>
       </c>
       <c r="F14" s="18">
         <v>1.768</v>
       </c>
-      <c r="G14" s="18">
-        <v>1.7210000000000001</v>
+      <c r="G14" s="68">
+        <v>2.7869999999999999</v>
       </c>
       <c r="H14" s="18">
-        <v>-4.7E-2</v>
+        <v>1.0189999999999999</v>
       </c>
       <c r="I14">
         <v>-14.290330000000001</v>
@@ -2551,29 +2593,31 @@
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B15" s="18">
         <v>114.633</v>
       </c>
-      <c r="C15" s="17"/>
+      <c r="C15" s="18">
+        <v>114.964</v>
+      </c>
       <c r="D15" s="18">
-        <v>-114.633</v>
-      </c>
-      <c r="E15" s="13" t="str">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="E15" s="67" t="str">
         <f t="shared" si="1"/>
         <v>P3A</v>
       </c>
       <c r="F15" s="18">
         <v>1.6679999999999999</v>
       </c>
-      <c r="G15" s="18">
-        <v>1.792</v>
+      <c r="G15" s="68">
+        <v>1.8169999999999999</v>
       </c>
       <c r="H15" s="18">
-        <v>0.124</v>
+        <v>0.14899999999999999</v>
       </c>
       <c r="I15">
         <v>-14.292730000000001</v>
@@ -2590,29 +2634,31 @@
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B16" s="18">
         <v>67.495000000000005</v>
       </c>
-      <c r="C16" s="17"/>
+      <c r="C16" s="18">
+        <v>67.531999999999996</v>
+      </c>
       <c r="D16" s="18">
-        <v>-67.495000000000005</v>
-      </c>
-      <c r="E16" s="13" t="str">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="E16" s="67" t="str">
         <f t="shared" si="1"/>
         <v>P3B</v>
       </c>
       <c r="F16" s="18">
         <v>1.681</v>
       </c>
-      <c r="G16" s="18">
-        <v>1.8759999999999999</v>
+      <c r="G16" s="68">
+        <v>1.724</v>
       </c>
       <c r="H16" s="18">
-        <v>0.19500000000000001</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="I16">
         <v>-14.293839999999999</v>
@@ -2629,29 +2675,31 @@
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B17" s="18">
         <v>68.353999999999999</v>
       </c>
-      <c r="C17" s="17"/>
+      <c r="C17" s="18">
+        <v>68.385999999999996</v>
+      </c>
       <c r="D17" s="18">
-        <v>-68.353999999999999</v>
-      </c>
-      <c r="E17" s="13" t="str">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="E17" s="67" t="str">
         <f t="shared" si="1"/>
         <v>P3C</v>
       </c>
       <c r="F17" s="18">
         <v>1.6910000000000001</v>
       </c>
-      <c r="G17" s="18">
-        <v>1.716</v>
+      <c r="G17" s="68">
+        <v>1.7070000000000001</v>
       </c>
       <c r="H17" s="18">
-        <v>2.5000000000000001E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="I17">
         <v>-14.293369999999999</v>
@@ -2673,34 +2721,36 @@
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
-      <c r="E18" s="13"/>
+      <c r="E18" s="67"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="18">
-        <v>68.125</v>
-      </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="18">
-        <v>-68.125</v>
-      </c>
-      <c r="E19" s="13" t="str">
+      <c r="B19" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="67" t="str">
         <f t="shared" si="1"/>
         <v>T1A</v>
       </c>
-      <c r="F19" s="18">
-        <v>1.653</v>
-      </c>
-      <c r="G19" s="18">
-        <v>2.9359999999999999</v>
-      </c>
-      <c r="H19" s="18">
-        <v>1.2829999999999999</v>
+      <c r="F19" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" s="18" t="s">
+        <v>24</v>
       </c>
       <c r="I19">
         <v>-14.290179999999999</v>
@@ -2717,29 +2767,31 @@
         <v>2.0268299163899908E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B20" s="18">
         <v>112.46299999999999</v>
       </c>
-      <c r="C20" s="17"/>
+      <c r="C20" s="18">
+        <v>118.566</v>
+      </c>
       <c r="D20" s="18">
-        <v>-112.46299999999999</v>
-      </c>
-      <c r="E20" s="13" t="str">
+        <v>6.1029999999999998</v>
+      </c>
+      <c r="E20" s="67" t="str">
         <f t="shared" si="1"/>
         <v>T1B</v>
       </c>
       <c r="F20" s="18">
         <v>1.6779999999999999</v>
       </c>
-      <c r="G20" s="18">
-        <v>4.3179999999999996</v>
+      <c r="G20" s="68">
+        <v>5.32</v>
       </c>
       <c r="H20" s="18">
-        <v>2.64</v>
+        <v>3.6419999999999999</v>
       </c>
       <c r="I20">
         <v>-14.28941</v>
@@ -2756,29 +2808,31 @@
         <v>2.0268299163899908E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="18">
         <v>66.397000000000006</v>
       </c>
-      <c r="C21" s="17"/>
+      <c r="C21" s="18">
+        <v>67.463999999999999</v>
+      </c>
       <c r="D21" s="18">
-        <v>-66.397000000000006</v>
-      </c>
-      <c r="E21" s="13" t="str">
+        <v>1.0669999999999999</v>
+      </c>
+      <c r="E21" s="67" t="str">
         <f t="shared" si="1"/>
         <v>T1C</v>
       </c>
       <c r="F21" s="18">
         <v>1.7090000000000001</v>
       </c>
-      <c r="G21" s="18">
-        <v>3.4740000000000002</v>
+      <c r="G21" s="68">
+        <v>2.06</v>
       </c>
       <c r="H21" s="18">
-        <v>1.7649999999999999</v>
+        <v>0.35099999999999998</v>
       </c>
       <c r="I21">
         <v>-14.28833</v>
@@ -2795,29 +2849,31 @@
         <v>2.0268299163899908E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B22" s="18">
         <v>70.290999999999997</v>
       </c>
-      <c r="C22" s="17"/>
+      <c r="C22" s="18">
+        <v>77.766999999999996</v>
+      </c>
       <c r="D22" s="18">
-        <v>-70.290999999999997</v>
-      </c>
-      <c r="E22" s="13" t="str">
+        <v>7.476</v>
+      </c>
+      <c r="E22" s="67" t="str">
         <f t="shared" si="1"/>
         <v>T2A</v>
       </c>
       <c r="F22" s="18">
         <v>1.6759999999999999</v>
       </c>
-      <c r="G22" s="18">
-        <v>7.093</v>
+      <c r="G22" s="68">
+        <v>3.8679999999999999</v>
       </c>
       <c r="H22" s="18">
-        <v>5.4169999999999998</v>
+        <v>2.1920000000000002</v>
       </c>
       <c r="I22">
         <v>-14.29177</v>
@@ -2834,29 +2890,31 @@
         <v>2.0268299163899908E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B23" s="18">
         <v>115.11</v>
       </c>
-      <c r="C23" s="17"/>
+      <c r="C23" s="18">
+        <v>115.119</v>
+      </c>
       <c r="D23" s="18">
-        <v>-115.11</v>
-      </c>
-      <c r="E23" s="13" t="str">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="E23" s="67" t="str">
         <f t="shared" si="1"/>
         <v>T2B</v>
       </c>
       <c r="F23" s="18">
         <v>1.728</v>
       </c>
-      <c r="G23" s="18">
-        <v>1.75</v>
+      <c r="G23" s="68">
+        <v>1.8149999999999999</v>
       </c>
       <c r="H23" s="18">
-        <v>2.1999999999999999E-2</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="I23">
         <v>-14.29142</v>
@@ -2873,29 +2931,31 @@
         <v>2.0268299163899908E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B24" s="18">
         <v>69.381</v>
       </c>
-      <c r="C24" s="17"/>
+      <c r="C24" s="18">
+        <v>70.066000000000003</v>
+      </c>
       <c r="D24" s="18">
-        <v>-69.381</v>
-      </c>
-      <c r="E24" s="13" t="str">
+        <v>0.68500000000000005</v>
+      </c>
+      <c r="E24" s="67" t="str">
         <f t="shared" si="1"/>
         <v>T2C</v>
       </c>
       <c r="F24" s="18">
         <v>1.746</v>
       </c>
-      <c r="G24" s="18">
-        <v>4.3550000000000004</v>
+      <c r="G24" s="68">
+        <v>3.8530000000000002</v>
       </c>
       <c r="H24" s="18">
-        <v>2.609</v>
+        <v>2.1070000000000002</v>
       </c>
       <c r="I24">
         <v>-14.290330000000001</v>
@@ -2912,29 +2972,31 @@
         <v>2.0268299163899908E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B25" s="18">
         <v>113.40300000000001</v>
       </c>
-      <c r="C25" s="17"/>
+      <c r="C25" s="18">
+        <v>113.651</v>
+      </c>
       <c r="D25" s="18">
-        <v>-113.40300000000001</v>
-      </c>
-      <c r="E25" s="13" t="str">
+        <v>0.248</v>
+      </c>
+      <c r="E25" s="67" t="str">
         <f t="shared" si="1"/>
         <v>T3A</v>
       </c>
       <c r="F25" s="18">
         <v>1.66</v>
       </c>
-      <c r="G25" s="18">
-        <v>2.3210000000000002</v>
+      <c r="G25" s="68">
+        <v>2.0219999999999998</v>
       </c>
       <c r="H25" s="18">
-        <v>0.66100000000000003</v>
+        <v>0.36199999999999999</v>
       </c>
       <c r="I25">
         <v>-14.292730000000001</v>
@@ -2951,29 +3013,31 @@
         <v>2.0268299163899908E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B26" s="18">
         <v>113.386</v>
       </c>
-      <c r="C26" s="17"/>
+      <c r="C26" s="18">
+        <v>113.798</v>
+      </c>
       <c r="D26" s="18">
-        <v>-113.386</v>
-      </c>
-      <c r="E26" s="13" t="str">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="E26" s="67" t="str">
         <f t="shared" si="1"/>
         <v>T3B</v>
       </c>
       <c r="F26" s="18">
         <v>1.706</v>
       </c>
-      <c r="G26" s="18">
-        <v>2.5979999999999999</v>
+      <c r="G26" s="68">
+        <v>2.254</v>
       </c>
       <c r="H26" s="18">
-        <v>0.89200000000000002</v>
+        <v>0.54800000000000004</v>
       </c>
       <c r="I26">
         <v>-14.293839999999999</v>
@@ -2990,29 +3054,31 @@
         <v>2.0268299163899908E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B27" s="18">
         <v>70.397999999999996</v>
       </c>
-      <c r="C27" s="17"/>
+      <c r="C27" s="18">
+        <v>70.492999999999995</v>
+      </c>
       <c r="D27" s="18">
-        <v>-70.397999999999996</v>
-      </c>
-      <c r="E27" s="13" t="str">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="E27" s="67" t="str">
         <f t="shared" si="1"/>
         <v>T3C</v>
       </c>
       <c r="F27" s="18">
         <v>1.6339999999999999</v>
       </c>
-      <c r="G27" s="18">
-        <v>1.7430000000000001</v>
+      <c r="G27" s="68">
+        <v>1.6839999999999999</v>
       </c>
       <c r="H27" s="18">
-        <v>0.109</v>
+        <v>0.05</v>
       </c>
       <c r="I27">
         <v>-14.293369999999999</v>
@@ -3041,10 +3107,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:H1048576"/>
+    <sheetView topLeftCell="A8" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3113,38 +3179,38 @@
       <c r="A7" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="66" t="s">
+      <c r="B7" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="66"/>
-      <c r="D7" s="66"/>
-      <c r="F7" s="66" t="s">
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
+      <c r="F7" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="66"/>
-      <c r="H7" s="66"/>
+      <c r="G7" s="69"/>
+      <c r="H7" s="69"/>
     </row>
     <row r="8" spans="1:12" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="31" t="s">
         <v>5</v>
       </c>
       <c r="E8" s="29"/>
-      <c r="F8" s="25" t="s">
+      <c r="F8" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="G8" s="25" t="s">
+      <c r="G8" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="H8" s="25" t="s">
+      <c r="H8" s="31" t="s">
         <v>6</v>
       </c>
       <c r="I8" s="32" t="s">
@@ -3160,18 +3226,20 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="18">
-        <v>70.528000000000006</v>
-      </c>
-      <c r="C9" s="17"/>
+      <c r="B9" s="68">
+        <v>2.4860000000000002</v>
+      </c>
+      <c r="C9" s="18">
+        <v>4.7279999999999998</v>
+      </c>
       <c r="D9" s="18">
-        <v>-70.528000000000006</v>
-      </c>
-      <c r="E9" s="13" t="str">
+        <v>2.242</v>
+      </c>
+      <c r="E9" s="67" t="str">
         <f>A9</f>
         <v>P1A</v>
       </c>
@@ -3191,7 +3259,7 @@
         <v>-170.6814</v>
       </c>
       <c r="K9">
-        <f t="shared" ref="K9:K17" si="0">$B$3-$B$2</f>
+        <f t="shared" ref="K9:K19" si="0">$B$3-$B$2</f>
         <v>30</v>
       </c>
       <c r="L9" s="14">
@@ -3199,19 +3267,21 @@
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="18">
-        <v>110.10599999999999</v>
-      </c>
-      <c r="C10" s="17"/>
+      <c r="B10" s="68">
+        <v>2.4809999999999999</v>
+      </c>
+      <c r="C10" s="18">
+        <v>6.7910000000000004</v>
+      </c>
       <c r="D10" s="18">
-        <v>-110.10599999999999</v>
-      </c>
-      <c r="E10" s="13" t="str">
-        <f t="shared" ref="E10:E27" si="1">A10</f>
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="E10" s="67" t="str">
+        <f t="shared" ref="E10:E31" si="1">A10</f>
         <v>P1B</v>
       </c>
       <c r="F10" s="18">
@@ -3238,18 +3308,20 @@
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="18">
-        <v>112.16200000000001</v>
-      </c>
-      <c r="C11" s="17"/>
+      <c r="B11" s="68">
+        <v>2.476</v>
+      </c>
+      <c r="C11" s="18">
+        <v>4.4800000000000004</v>
+      </c>
       <c r="D11" s="18">
-        <v>-112.16200000000001</v>
-      </c>
-      <c r="E11" s="13" t="str">
+        <v>2.004</v>
+      </c>
+      <c r="E11" s="67" t="str">
         <f t="shared" si="1"/>
         <v>P1C</v>
       </c>
@@ -3279,18 +3351,14 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="18">
-        <v>69.935000000000002</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="B12" s="18"/>
       <c r="C12" s="17"/>
-      <c r="D12" s="18">
-        <v>-69.935000000000002</v>
-      </c>
-      <c r="E12" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>P2A</v>
+      <c r="D12" s="18"/>
+      <c r="E12" s="67" t="str">
+        <f t="shared" si="1"/>
+        <v>P2A-a</v>
       </c>
       <c r="F12" s="18">
         <v>1.6379999999999999</v>
@@ -3318,72 +3386,51 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="18">
-        <v>113.377</v>
-      </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="18">
-        <v>-113.377</v>
-      </c>
-      <c r="E13" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>P2B</v>
+        <v>76</v>
+      </c>
+      <c r="E13" s="67" t="str">
+        <f t="shared" si="1"/>
+        <v>P2A-b</v>
       </c>
       <c r="F13" s="18">
-        <v>1.681</v>
+        <v>1.6819999999999999</v>
       </c>
       <c r="G13" s="18">
-        <v>1.7130000000000001</v>
+        <v>6.22</v>
       </c>
       <c r="H13" s="18">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="I13">
-        <v>-14.29142</v>
-      </c>
-      <c r="J13">
-        <v>-170.67930000000001</v>
-      </c>
-      <c r="K13">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="L13" s="14">
-        <f>Mar_2014!$I$2</f>
-        <v>1.8241469247509915E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>4.5380000000000003</v>
+      </c>
+      <c r="L13" s="14"/>
+    </row>
+    <row r="14" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="18">
-        <v>67.063000000000002</v>
-      </c>
-      <c r="C14" s="17"/>
+        <v>34</v>
+      </c>
+      <c r="B14" s="68">
+        <v>2.5070000000000001</v>
+      </c>
+      <c r="C14" s="18">
+        <v>10.756</v>
+      </c>
       <c r="D14" s="18">
-        <v>-67.063000000000002</v>
-      </c>
-      <c r="E14" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>P2C</v>
-      </c>
-      <c r="F14" s="18">
-        <v>1.6950000000000001</v>
-      </c>
-      <c r="G14" s="18">
-        <v>1.7210000000000001</v>
-      </c>
+        <v>8.2490000000000006</v>
+      </c>
+      <c r="E14" s="67" t="str">
+        <f t="shared" si="1"/>
+        <v>P2A</v>
+      </c>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
       <c r="H14" s="18">
-        <v>2.5999999999999999E-2</v>
+        <f>H12+H13</f>
+        <v>9.5519999999999996</v>
       </c>
       <c r="I14">
-        <v>-14.290330000000001</v>
+        <v>-14.29177</v>
       </c>
       <c r="J14">
-        <v>-170.67670000000001</v>
+        <v>-170.68219999999999</v>
       </c>
       <c r="K14">
         <f t="shared" si="0"/>
@@ -3394,35 +3441,37 @@
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="18">
-        <v>114.633</v>
-      </c>
-      <c r="C15" s="17"/>
+        <v>35</v>
+      </c>
+      <c r="B15" s="68">
+        <v>2.5009999999999999</v>
+      </c>
+      <c r="C15" s="18">
+        <v>2.6709999999999998</v>
+      </c>
       <c r="D15" s="18">
-        <v>-114.633</v>
-      </c>
-      <c r="E15" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>P3A</v>
+        <v>0.17</v>
+      </c>
+      <c r="E15" s="67" t="str">
+        <f t="shared" si="1"/>
+        <v>P2B</v>
       </c>
       <c r="F15" s="18">
-        <v>1.631</v>
+        <v>1.681</v>
       </c>
       <c r="G15" s="18">
-        <v>1.792</v>
+        <v>1.7130000000000001</v>
       </c>
       <c r="H15" s="18">
-        <v>0.161</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="I15">
-        <v>-14.292730000000001</v>
+        <v>-14.29142</v>
       </c>
       <c r="J15">
-        <v>-170.67939999999999</v>
+        <v>-170.67930000000001</v>
       </c>
       <c r="K15">
         <f t="shared" si="0"/>
@@ -3433,35 +3482,37 @@
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="18">
-        <v>67.495000000000005</v>
-      </c>
-      <c r="C16" s="17"/>
+        <v>36</v>
+      </c>
+      <c r="B16" s="68">
+        <v>2.476</v>
+      </c>
+      <c r="C16" s="18">
+        <v>3.7080000000000002</v>
+      </c>
       <c r="D16" s="18">
-        <v>-67.495000000000005</v>
-      </c>
-      <c r="E16" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>P3B</v>
+        <v>1.232</v>
+      </c>
+      <c r="E16" s="67" t="str">
+        <f t="shared" si="1"/>
+        <v>P2C</v>
       </c>
       <c r="F16" s="18">
-        <v>1.653</v>
+        <v>1.6950000000000001</v>
       </c>
       <c r="G16" s="18">
-        <v>1.8759999999999999</v>
+        <v>1.7210000000000001</v>
       </c>
       <c r="H16" s="18">
-        <v>0.223</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="I16">
-        <v>-14.293839999999999</v>
+        <v>-14.290330000000001</v>
       </c>
       <c r="J16">
-        <v>-170.6773</v>
+        <v>-170.67670000000001</v>
       </c>
       <c r="K16">
         <f t="shared" si="0"/>
@@ -3472,35 +3523,37 @@
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="18">
-        <v>68.353999999999999</v>
-      </c>
-      <c r="C17" s="17"/>
+        <v>30</v>
+      </c>
+      <c r="B17" s="68">
+        <v>2.52</v>
+      </c>
+      <c r="C17" s="18">
+        <v>2.7759999999999998</v>
+      </c>
       <c r="D17" s="18">
-        <v>-68.353999999999999</v>
-      </c>
-      <c r="E17" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>P3C</v>
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="E17" s="67" t="str">
+        <f t="shared" si="1"/>
+        <v>P3A</v>
       </c>
       <c r="F17" s="18">
-        <v>1.7110000000000001</v>
+        <v>1.631</v>
       </c>
       <c r="G17" s="18">
-        <v>1.716</v>
+        <v>1.792</v>
       </c>
       <c r="H17" s="18">
-        <v>5.0000000000000001E-3</v>
+        <v>0.161</v>
       </c>
       <c r="I17">
-        <v>-14.293369999999999</v>
+        <v>-14.292730000000001</v>
       </c>
       <c r="J17">
-        <v>-170.6754</v>
+        <v>-170.67939999999999</v>
       </c>
       <c r="K17">
         <f t="shared" si="0"/>
@@ -3511,126 +3564,132 @@
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="68">
+        <v>2.5259999999999998</v>
+      </c>
+      <c r="C18" s="18">
+        <v>2.5630000000000002</v>
+      </c>
+      <c r="D18" s="18">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="E18" s="67" t="str">
+        <f t="shared" si="1"/>
+        <v>P3B</v>
+      </c>
+      <c r="F18" s="18">
+        <v>1.653</v>
+      </c>
+      <c r="G18" s="18">
+        <v>1.8759999999999999</v>
+      </c>
+      <c r="H18" s="18">
+        <v>0.223</v>
+      </c>
+      <c r="I18">
+        <v>-14.293839999999999</v>
+      </c>
+      <c r="J18">
+        <v>-170.6773</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="L18" s="14">
+        <f>Mar_2014!$I$2</f>
+        <v>1.8241469247509915E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="68">
+        <v>2.5230000000000001</v>
+      </c>
+      <c r="C19" s="18">
+        <v>2.54</v>
+      </c>
+      <c r="D19" s="18">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="E19" s="67" t="str">
+        <f t="shared" si="1"/>
+        <v>P3C</v>
+      </c>
+      <c r="F19" s="18">
+        <v>1.7110000000000001</v>
+      </c>
+      <c r="G19" s="18">
+        <v>1.716</v>
+      </c>
+      <c r="H19" s="18">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="I19">
+        <v>-14.293369999999999</v>
+      </c>
+      <c r="J19">
+        <v>-170.6754</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="L19" s="14">
+        <f>Mar_2014!$I$2</f>
+        <v>1.8241469247509915E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" spans="1:12" ht="30.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="18">
-        <v>68.125</v>
-      </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="18">
-        <v>-68.125</v>
-      </c>
-      <c r="E19" s="13" t="str">
+      <c r="B21" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="67" t="str">
         <f t="shared" si="1"/>
         <v>T1A</v>
       </c>
-      <c r="F19" s="18">
-        <v>1.673</v>
-      </c>
-      <c r="G19" s="18">
-        <v>2.9359999999999999</v>
-      </c>
-      <c r="H19" s="18">
-        <v>1.2629999999999999</v>
-      </c>
-      <c r="I19">
+      <c r="F21" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="H21" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="I21">
         <v>-14.290179999999999</v>
       </c>
-      <c r="J19">
+      <c r="J21">
         <v>-170.6814</v>
       </c>
-      <c r="K19">
-        <f t="shared" ref="K19:K27" si="2">$B$3-$B$2</f>
-        <v>30</v>
-      </c>
-      <c r="L19" s="14">
-        <f>Mar_2014!$I$3</f>
-        <v>2.0268299163899908E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" s="18">
-        <v>112.46299999999999</v>
-      </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="18">
-        <v>-112.46299999999999</v>
-      </c>
-      <c r="E20" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>T1B</v>
-      </c>
-      <c r="F20" s="18">
-        <v>1.627</v>
-      </c>
-      <c r="G20" s="18">
-        <v>4.3179999999999996</v>
-      </c>
-      <c r="H20" s="18">
-        <v>2.6909999999999998</v>
-      </c>
-      <c r="I20">
-        <v>-14.28941</v>
-      </c>
-      <c r="J20">
-        <v>-170.67959999999999</v>
-      </c>
-      <c r="K20">
-        <f t="shared" si="2"/>
-        <v>30</v>
-      </c>
-      <c r="L20" s="14">
-        <f>Mar_2014!$I$3</f>
-        <v>2.0268299163899908E-3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="18">
-        <v>66.397000000000006</v>
-      </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="18">
-        <v>-66.397000000000006</v>
-      </c>
-      <c r="E21" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>T1C</v>
-      </c>
-      <c r="F21" s="18">
-        <v>1.6830000000000001</v>
-      </c>
-      <c r="G21" s="18">
-        <v>3.4740000000000002</v>
-      </c>
-      <c r="H21" s="18">
-        <v>1.7909999999999999</v>
-      </c>
-      <c r="I21">
-        <v>-14.28833</v>
-      </c>
-      <c r="J21">
-        <v>-170.67789999999999</v>
-      </c>
       <c r="K21">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="K21:K31" si="2">$B$3-$B$2</f>
         <v>30</v>
       </c>
       <c r="L21" s="14">
@@ -3638,113 +3697,78 @@
         <v>2.0268299163899908E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B22" s="18">
-        <v>70.290999999999997</v>
-      </c>
-      <c r="C22" s="17"/>
-      <c r="D22" s="18">
-        <v>-70.290999999999997</v>
-      </c>
-      <c r="E22" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>T2A</v>
+        <v>77</v>
+      </c>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="67" t="str">
+        <f t="shared" si="1"/>
+        <v>T1B-a</v>
       </c>
       <c r="F22" s="18">
         <v>1.6779999999999999</v>
       </c>
-      <c r="G22" s="18">
-        <v>7.093</v>
+      <c r="G22" s="68">
+        <v>6.3970000000000002</v>
       </c>
       <c r="H22" s="18">
-        <v>5.415</v>
-      </c>
-      <c r="I22">
-        <v>-14.29177</v>
-      </c>
-      <c r="J22">
-        <v>-170.68219999999999</v>
-      </c>
-      <c r="K22">
-        <f t="shared" si="2"/>
-        <v>30</v>
-      </c>
-      <c r="L22" s="14">
-        <f>Mar_2014!$I$3</f>
-        <v>2.0268299163899908E-3</v>
-      </c>
+        <v>4.7190000000000003</v>
+      </c>
+      <c r="L22" s="14"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" s="18">
-        <v>115.11</v>
-      </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="18">
-        <v>-115.11</v>
-      </c>
-      <c r="E23" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>T2B</v>
+        <v>78</v>
+      </c>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="67" t="str">
+        <f t="shared" si="1"/>
+        <v>T1B-b</v>
       </c>
       <c r="F23" s="18">
-        <v>1.667</v>
-      </c>
-      <c r="G23" s="18">
-        <v>1.75</v>
+        <v>1.653</v>
+      </c>
+      <c r="G23" s="16">
+        <v>4.8170000000000002</v>
       </c>
       <c r="H23" s="18">
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="I23">
-        <v>-14.29142</v>
-      </c>
-      <c r="J23">
-        <v>-170.67930000000001</v>
-      </c>
-      <c r="K23">
-        <f t="shared" si="2"/>
-        <v>30</v>
-      </c>
-      <c r="L23" s="14">
-        <f>Mar_2014!$I$3</f>
-        <v>2.0268299163899908E-3</v>
-      </c>
+        <v>3.1640000000000001</v>
+      </c>
+      <c r="L23" s="14"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B24" s="18">
-        <v>69.381</v>
-      </c>
-      <c r="C24" s="17"/>
+        <v>2.4849999999999999</v>
+      </c>
+      <c r="C24" s="18">
+        <v>17.739999999999998</v>
+      </c>
       <c r="D24" s="18">
-        <v>-69.381</v>
-      </c>
-      <c r="E24" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>T2C</v>
-      </c>
-      <c r="F24" s="18">
-        <v>1.6679999999999999</v>
-      </c>
-      <c r="G24" s="18">
-        <v>4.3550000000000004</v>
-      </c>
+        <v>15.255000000000001</v>
+      </c>
+      <c r="E24" s="67" t="str">
+        <f t="shared" si="1"/>
+        <v>T1B</v>
+      </c>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
       <c r="H24" s="18">
-        <v>2.6869999999999998</v>
+        <f>H22+H23</f>
+        <v>7.8830000000000009</v>
       </c>
       <c r="I24">
-        <v>-14.290330000000001</v>
+        <v>-14.28941</v>
       </c>
       <c r="J24">
-        <v>-170.67670000000001</v>
+        <v>-170.67959999999999</v>
       </c>
       <c r="K24">
         <f t="shared" si="2"/>
@@ -3755,35 +3779,37 @@
         <v>2.0268299163899908E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B25" s="18">
-        <v>113.40300000000001</v>
-      </c>
-      <c r="C25" s="17"/>
+        <v>16</v>
+      </c>
+      <c r="B25" s="68">
+        <v>2.488</v>
+      </c>
+      <c r="C25" s="18">
+        <v>3.8149999999999999</v>
+      </c>
       <c r="D25" s="18">
-        <v>-113.40300000000001</v>
-      </c>
-      <c r="E25" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>T3A</v>
+        <v>1.327</v>
+      </c>
+      <c r="E25" s="67" t="str">
+        <f t="shared" si="1"/>
+        <v>T1C</v>
       </c>
       <c r="F25" s="18">
-        <v>1.639</v>
-      </c>
-      <c r="G25" s="18">
-        <v>2.3210000000000002</v>
+        <v>1.71</v>
+      </c>
+      <c r="G25" s="68">
+        <v>4.8410000000000002</v>
       </c>
       <c r="H25" s="18">
-        <v>0.68200000000000005</v>
+        <v>3.1309999999999998</v>
       </c>
       <c r="I25">
-        <v>-14.292730000000001</v>
+        <v>-14.28833</v>
       </c>
       <c r="J25">
-        <v>-170.67939999999999</v>
+        <v>-170.67789999999999</v>
       </c>
       <c r="K25">
         <f t="shared" si="2"/>
@@ -3794,33 +3820,37 @@
         <v>2.0268299163899908E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" s="18">
-        <v>113.386</v>
-      </c>
-      <c r="C26" s="17"/>
+        <v>10</v>
+      </c>
+      <c r="B26" s="68">
+        <v>2.4969999999999999</v>
+      </c>
+      <c r="C26" s="18">
+        <v>3.0129999999999999</v>
+      </c>
       <c r="D26" s="18">
-        <v>-113.386</v>
-      </c>
-      <c r="E26" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>T3B</v>
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="E26" s="67" t="str">
+        <f t="shared" si="1"/>
+        <v>T2A</v>
       </c>
       <c r="F26" s="18">
-        <v>1.71</v>
-      </c>
-      <c r="G26" s="17"/>
+        <v>1.639</v>
+      </c>
+      <c r="G26" s="68">
+        <v>12.705</v>
+      </c>
       <c r="H26" s="18">
-        <v>-1.71</v>
+        <v>11.066000000000001</v>
       </c>
       <c r="I26">
-        <v>-14.293839999999999</v>
+        <v>-14.29177</v>
       </c>
       <c r="J26">
-        <v>-170.6773</v>
+        <v>-170.68219999999999</v>
       </c>
       <c r="K26">
         <f t="shared" si="2"/>
@@ -3831,41 +3861,207 @@
         <v>2.0268299163899908E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B27" s="18">
-        <v>70.397999999999996</v>
-      </c>
-      <c r="C27" s="17"/>
+        <v>15</v>
+      </c>
+      <c r="B27" s="68">
+        <v>2.4780000000000002</v>
+      </c>
+      <c r="C27" s="18">
+        <v>3.0870000000000002</v>
+      </c>
       <c r="D27" s="18">
-        <v>-70.397999999999996</v>
-      </c>
-      <c r="E27" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>T3C</v>
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="E27" s="67" t="str">
+        <f t="shared" si="1"/>
+        <v>T2B</v>
       </c>
       <c r="F27" s="18">
-        <v>1.6679999999999999</v>
-      </c>
-      <c r="G27" s="18">
-        <v>1.7430000000000001</v>
+        <v>1.6779999999999999</v>
+      </c>
+      <c r="G27" s="68">
+        <v>2.8420000000000001</v>
       </c>
       <c r="H27" s="18">
-        <v>7.4999999999999997E-2</v>
+        <v>1.1639999999999999</v>
       </c>
       <c r="I27">
-        <v>-14.293369999999999</v>
+        <v>-14.29142</v>
       </c>
       <c r="J27">
-        <v>-170.6754</v>
+        <v>-170.67930000000001</v>
       </c>
       <c r="K27">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="L27" s="14">
+        <f>Mar_2014!$I$3</f>
+        <v>2.0268299163899908E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="68">
+        <v>2.5009999999999999</v>
+      </c>
+      <c r="C28" s="18">
+        <v>4.13</v>
+      </c>
+      <c r="D28" s="18">
+        <v>1.629</v>
+      </c>
+      <c r="E28" s="67" t="str">
+        <f t="shared" si="1"/>
+        <v>T2C</v>
+      </c>
+      <c r="F28" s="18">
+        <v>1.6679999999999999</v>
+      </c>
+      <c r="G28" s="68">
+        <v>5.23</v>
+      </c>
+      <c r="H28" s="18">
+        <v>3.5619999999999998</v>
+      </c>
+      <c r="I28">
+        <v>-14.290330000000001</v>
+      </c>
+      <c r="J28">
+        <v>-170.67670000000001</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="L28" s="14">
+        <f>Mar_2014!$I$3</f>
+        <v>2.0268299163899908E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" s="68">
+        <v>2.4870000000000001</v>
+      </c>
+      <c r="C29" s="18">
+        <v>3.8069999999999999</v>
+      </c>
+      <c r="D29" s="18">
+        <v>1.32</v>
+      </c>
+      <c r="E29" s="67" t="str">
+        <f t="shared" si="1"/>
+        <v>T3A</v>
+      </c>
+      <c r="F29" s="18">
+        <v>1.627</v>
+      </c>
+      <c r="G29" s="68">
+        <v>3.133</v>
+      </c>
+      <c r="H29" s="18">
+        <v>1.506</v>
+      </c>
+      <c r="I29">
+        <v>-14.292730000000001</v>
+      </c>
+      <c r="J29">
+        <v>-170.67939999999999</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="L29" s="14">
+        <f>Mar_2014!$I$3</f>
+        <v>2.0268299163899908E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="68">
+        <v>2.484</v>
+      </c>
+      <c r="C30" s="18">
+        <v>2.6240000000000001</v>
+      </c>
+      <c r="D30" s="18">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E30" s="67" t="str">
+        <f t="shared" si="1"/>
+        <v>T3B</v>
+      </c>
+      <c r="F30" s="18">
+        <v>1.667</v>
+      </c>
+      <c r="G30" s="68">
+        <v>4.3579999999999997</v>
+      </c>
+      <c r="H30" s="18">
+        <v>2.6909999999999998</v>
+      </c>
+      <c r="I30">
+        <v>-14.293839999999999</v>
+      </c>
+      <c r="J30">
+        <v>-170.6773</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="L30" s="14">
+        <f>Mar_2014!$I$3</f>
+        <v>2.0268299163899908E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="68">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="C31" s="18">
+        <v>2.84</v>
+      </c>
+      <c r="D31" s="18">
+        <v>0.37</v>
+      </c>
+      <c r="E31" s="67" t="str">
+        <f t="shared" si="1"/>
+        <v>T3C</v>
+      </c>
+      <c r="F31" s="18">
+        <v>1.6830000000000001</v>
+      </c>
+      <c r="G31" s="68">
+        <v>1.8109999999999999</v>
+      </c>
+      <c r="H31" s="18">
+        <v>0.128</v>
+      </c>
+      <c r="I31">
+        <v>-14.293369999999999</v>
+      </c>
+      <c r="J31">
+        <v>-170.6754</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="L31" s="14">
         <f>Mar_2014!$I$3</f>
         <v>2.0268299163899908E-3</v>
       </c>
@@ -3949,16 +4145,16 @@
       <c r="A7" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="66" t="s">
+      <c r="B7" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="66"/>
-      <c r="D7" s="66"/>
-      <c r="F7" s="66" t="s">
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
+      <c r="F7" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="66"/>
-      <c r="H7" s="66"/>
+      <c r="G7" s="69"/>
+      <c r="H7" s="69"/>
     </row>
     <row r="8" spans="1:12" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
@@ -4740,7 +4936,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
@@ -4805,16 +5001,16 @@
       <c r="A7" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="66" t="s">
+      <c r="B7" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="66"/>
-      <c r="D7" s="66"/>
-      <c r="F7" s="66" t="s">
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
+      <c r="F7" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="66"/>
-      <c r="H7" s="66"/>
+      <c r="G7" s="69"/>
+      <c r="H7" s="69"/>
     </row>
     <row r="8" spans="1:12" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
@@ -5600,8 +5796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5664,16 +5860,16 @@
       <c r="A7" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="67"/>
-      <c r="D7" s="67"/>
-      <c r="F7" s="67" t="s">
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
+      <c r="F7" s="70" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="67"/>
-      <c r="H7" s="67"/>
+      <c r="G7" s="70"/>
+      <c r="H7" s="70"/>
     </row>
     <row r="8" spans="1:12" s="41" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="37" t="s">
@@ -6707,16 +6903,16 @@
       <c r="A7" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="68" t="s">
+      <c r="B7" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="68"/>
-      <c r="D7" s="68"/>
-      <c r="F7" s="68" t="s">
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
+      <c r="F7" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="68"/>
-      <c r="H7" s="68"/>
+      <c r="G7" s="71"/>
+      <c r="H7" s="71"/>
     </row>
     <row r="8" spans="1:12" s="60" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="57" t="s">
@@ -7792,16 +7988,16 @@
       <c r="A7" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="66" t="s">
+      <c r="B7" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="66"/>
-      <c r="D7" s="66"/>
-      <c r="F7" s="66" t="s">
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
+      <c r="F7" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="66"/>
-      <c r="H7" s="66"/>
+      <c r="G7" s="69"/>
+      <c r="H7" s="69"/>
     </row>
     <row r="8" spans="1:12" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
@@ -8634,7 +8830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
       <selection activeCell="B10" sqref="B10:D10"/>
     </sheetView>
   </sheetViews>
@@ -8702,16 +8898,16 @@
       <c r="A7" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="66" t="s">
+      <c r="B7" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="66"/>
-      <c r="D7" s="66"/>
-      <c r="F7" s="66" t="s">
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
+      <c r="F7" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="66"/>
-      <c r="H7" s="66"/>
+      <c r="G7" s="69"/>
+      <c r="H7" s="69"/>
     </row>
     <row r="8" spans="1:12" s="20" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
@@ -8846,7 +9042,7 @@
         <v>69.652000000000001</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" ref="D10:D16" si="3">C11-B11</f>
+        <f t="shared" ref="D11:D16" si="3">C11-B11</f>
         <v>1.5810000000000031</v>
       </c>
       <c r="E11" s="13" t="str">
@@ -9612,16 +9808,16 @@
       <c r="A7" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="66" t="s">
+      <c r="B7" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="66"/>
-      <c r="D7" s="66"/>
-      <c r="F7" s="66" t="s">
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
+      <c r="F7" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="66"/>
-      <c r="H7" s="66"/>
+      <c r="G7" s="69"/>
+      <c r="H7" s="69"/>
     </row>
     <row r="8" spans="1:12" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
@@ -10418,7 +10614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -10488,16 +10684,16 @@
       <c r="A7" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="66" t="s">
+      <c r="B7" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="66"/>
-      <c r="D7" s="66"/>
-      <c r="F7" s="66" t="s">
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
+      <c r="F7" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="66"/>
-      <c r="H7" s="66"/>
+      <c r="G7" s="69"/>
+      <c r="H7" s="69"/>
     </row>
     <row r="8" spans="1:12" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">

</xml_diff>

<commit_message>
2014 data in and plotted
looks good methinks
</commit_message>
<xml_diff>
--- a/Data/CRCP Sediment Data Bulk Weight and Composition.xlsx
+++ b/Data/CRCP Sediment Data Bulk Weight and Composition.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" tabRatio="500" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" tabRatio="500" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Mar_2014" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="79">
   <si>
     <t>Pod(P)/Tube(T)</t>
   </si>
@@ -997,8 +997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F16" sqref="F15:H16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2230,7 +2230,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+    <sheetView zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
       <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
@@ -3109,8 +3109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A4" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4081,7 +4081,7 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4936,8 +4936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5796,7 +5796,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
@@ -6825,7 +6825,7 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7908,7 +7908,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -8830,8 +8830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:D10"/>
+    <sheetView zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -9299,8 +9299,8 @@
       <c r="C17" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D17" s="1">
-        <v>0</v>
+      <c r="D17" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="E17" s="13" t="str">
         <f t="shared" si="2"/>
@@ -9312,8 +9312,8 @@
       <c r="G17" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="H17" s="1">
-        <v>0</v>
+      <c r="H17" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="I17">
         <v>-14.293369999999999</v>
@@ -9522,8 +9522,8 @@
       <c r="C23" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D23" s="1">
-        <v>0</v>
+      <c r="D23" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="E23" s="13" t="str">
         <f t="shared" si="2"/>
@@ -9535,8 +9535,8 @@
       <c r="G23" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="H23" s="1">
-        <v>0</v>
+      <c r="H23" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="I23">
         <v>-14.29142</v>
@@ -9739,7 +9739,7 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="F23" sqref="F23:H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -10193,8 +10193,8 @@
       <c r="C17" s="16">
         <v>100.636</v>
       </c>
-      <c r="D17" s="16">
-        <v>0</v>
+      <c r="D17" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="E17" s="13" t="str">
         <f t="shared" si="1"/>
@@ -10403,23 +10403,27 @@
       <c r="A23" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="17"/>
-      <c r="C23" s="16">
-        <v>0</v>
-      </c>
-      <c r="D23" s="16">
-        <v>0</v>
+      <c r="B23" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="E23" s="13" t="str">
         <f t="shared" si="1"/>
         <v>T2B</v>
       </c>
-      <c r="F23" s="17"/>
-      <c r="G23" s="16">
-        <v>0</v>
-      </c>
-      <c r="H23" s="16">
-        <v>0</v>
+      <c r="F23" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="I23">
         <v>-14.29142</v>
@@ -10614,7 +10618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
plotted SedPods v Tubes
</commit_message>
<xml_diff>
--- a/Data/CRCP Sediment Data Bulk Weight and Composition.xlsx
+++ b/Data/CRCP Sediment Data Bulk Weight and Composition.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" tabRatio="500" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Mar_2014" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="Feb_2015" sheetId="13" r:id="rId10"/>
     <sheet name="Mar_2015" sheetId="14" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -997,7 +997,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
@@ -3109,7 +3109,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+    <sheetView zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
       <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
@@ -7908,7 +7908,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+    <sheetView zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
had to change the regression method
bad p values using sm.OLS; some issue with the intercept?
</commit_message>
<xml_diff>
--- a/Data/CRCP Sediment Data Bulk Weight and Composition.xlsx
+++ b/Data/CRCP Sediment Data Bulk Weight and Composition.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" tabRatio="654"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" tabRatio="654" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Test_2015" sheetId="16" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="80">
   <si>
     <t>Pod(P)/Tube(T)</t>
   </si>
@@ -268,6 +268,9 @@
   <si>
     <t>T1B-b</t>
   </si>
+  <si>
+    <t>** Lab results for T1B on this month show zero sediment but that has to be an error</t>
+  </si>
 </sst>
 </file>
 
@@ -278,9 +281,16 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -482,35 +492,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -552,85 +562,126 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -998,7 +1049,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+    <sheetView zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
@@ -1080,7 +1131,7 @@
       <c r="G7" s="69"/>
       <c r="H7" s="69"/>
     </row>
-    <row r="8" spans="1:12" s="20" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" s="20" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
         <v>0</v>
       </c>
@@ -6736,7 +6787,7 @@
     <mergeCell ref="F7:H7"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D9 H1:H9 H11:H16 D11:D16 D18:D1048576 H18:H1048576">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7596,7 +7647,7 @@
     <mergeCell ref="F7:H7"/>
   </mergeCells>
   <conditionalFormatting sqref="D1 H1:H1048576 D3:D1048576">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7606,10 +7657,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8036,7 +8087,7 @@
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="42" t="s">
         <v>38</v>
       </c>
@@ -8075,7 +8126,7 @@
         <v>1.8241469247509915E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="48"/>
       <c r="B18" s="48"/>
       <c r="C18" s="48"/>
@@ -8085,7 +8136,7 @@
       <c r="G18" s="48"/>
       <c r="H18" s="48"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="42" t="s">
         <v>13</v>
       </c>
@@ -8125,30 +8176,28 @@
         <v>2.0268299163899908E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="42">
-        <v>66.369600000000005</v>
-      </c>
-      <c r="C20" s="42">
-        <v>66.436099999999996</v>
-      </c>
-      <c r="D20" s="43">
-        <f t="shared" si="3"/>
-        <v>6.6499999999990678E-2</v>
+      <c r="B20" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="42" t="s">
+        <v>24</v>
       </c>
       <c r="E20" s="44"/>
-      <c r="F20" s="45">
-        <v>1.7941</v>
-      </c>
-      <c r="G20" s="42">
-        <v>1.7761</v>
-      </c>
-      <c r="H20" s="42">
-        <f t="shared" si="4"/>
-        <v>-1.8000000000000016E-2</v>
+      <c r="F20" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="H20" s="42" t="s">
+        <v>24</v>
       </c>
       <c r="I20" s="34">
         <v>-14.28941</v>
@@ -8164,8 +8213,11 @@
         <f>Mar_2014!$I$3</f>
         <v>2.0268299163899908E-3</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M20" s="73" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="42" t="s">
         <v>16</v>
       </c>
@@ -8205,7 +8257,7 @@
         <v>2.0268299163899908E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="42" t="s">
         <v>44</v>
       </c>
@@ -8232,7 +8284,7 @@
       </c>
       <c r="L22" s="46"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="42" t="s">
         <v>45</v>
       </c>
@@ -8259,7 +8311,7 @@
       </c>
       <c r="L23" s="46"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="42" t="s">
         <v>46</v>
       </c>
@@ -8286,7 +8338,7 @@
       </c>
       <c r="L24" s="46"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="42" t="s">
         <v>47</v>
       </c>
@@ -8313,7 +8365,7 @@
       </c>
       <c r="L25" s="46"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="42" t="s">
         <v>48</v>
       </c>
@@ -8340,7 +8392,7 @@
       </c>
       <c r="L26" s="46"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="42" t="s">
         <v>10</v>
       </c>
@@ -8372,7 +8424,7 @@
         <v>2.0268299163899908E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="42" t="s">
         <v>15</v>
       </c>
@@ -8412,7 +8464,7 @@
         <v>2.0268299163899908E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="42" t="s">
         <v>8</v>
       </c>
@@ -8452,7 +8504,7 @@
         <v>2.0268299163899908E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="42" t="s">
         <v>11</v>
       </c>
@@ -8492,7 +8544,7 @@
         <v>2.0268299163899908E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="42" t="s">
         <v>7</v>
       </c>
@@ -8532,7 +8584,7 @@
         <v>2.0268299163899908E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="42" t="s">
         <v>12</v>
       </c>
@@ -8622,8 +8674,18 @@
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="F7:H7"/>
   </mergeCells>
-  <conditionalFormatting sqref="D1 H1:H15 D3:D1048576 H18:H1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+  <conditionalFormatting sqref="D1 H1:H15 D3:D19 H18:H19 D21:D1048576 H21:H1048576">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D20">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H20">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>